<commit_message>
add zone base firewall
</commit_message>
<xml_diff>
--- a/code/ip.xlsx
+++ b/code/ip.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="257">
   <si>
     <t>子网1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -627,6 +627,294 @@
   </si>
   <si>
     <t>为核心交换所使用端口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vlan号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vlan名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可用ip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网关设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>guke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>neike</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waike</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pifu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>erke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhongyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.0.32-63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.0.64-95</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.0.96-127</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.0.128-159</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.0.160-191</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.0.192-223</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.0.224-255</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yanke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.2.160-191</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.2.192-223</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.2.224-255</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fuchan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kouqiang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>erbi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tengtong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhongliu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shenwai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shennei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.0.1-31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>子网掩码为255.255.255.252，每个子网只有两台主机可用,主要用于上层三层连接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个子网容纳30台主机，子网掩码为255.255.255.224</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yibaoban</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yiwuke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>caiwuke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.3.32-63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.3.64-95</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.3.96-127</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>huyan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bchao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>suishi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cti</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.1.1-31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.1.32-63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.1.64-95</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.1.96-127</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.1.128-159</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.1.160-191</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.1.192-223</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.1.224-255</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.2.1-31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.2.32-63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.2.64-95</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.2.96-127</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.2.128-159</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.4.32-63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.4.64-95</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.4.96-127</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>172.16.4.128-159</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yingyang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quankemen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>teyuemen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaowuzixun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yingxiang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kangfuke</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heyixue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gaoyayang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xinshenyi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gonghui</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>门诊部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>行政部门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>医技楼</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -659,12 +947,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -673,8 +976,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -978,13 +1284,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="17.625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
@@ -1716,6 +2025,457 @@
       <c r="C75" t="s">
         <v>184</v>
       </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A79" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A80" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A81" s="1">
+        <v>2</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A82" s="1">
+        <v>3</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A83" s="1">
+        <v>4</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A84" s="1">
+        <v>5</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A85" s="1">
+        <v>6</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A86" s="1">
+        <v>7</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A87" s="1">
+        <v>8</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A88" s="1">
+        <v>9</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A89" s="1">
+        <v>10</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A90" s="1">
+        <v>11</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A91" s="1">
+        <v>12</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A92" s="1">
+        <v>13</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A93" s="1">
+        <v>14</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A94" s="1">
+        <v>15</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A95" s="1">
+        <v>16</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A96" s="1">
+        <v>17</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A97" s="1">
+        <v>18</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A98" s="1">
+        <v>19</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A99" s="1">
+        <v>20</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A100" s="1">
+        <v>21</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A101" s="1">
+        <v>22</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A102" s="1">
+        <v>23</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A103" s="1">
+        <v>24</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A104" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A105" s="1">
+        <v>25</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A106" s="1">
+        <v>26</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A107" s="1">
+        <v>27</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A108" s="1">
+        <v>28</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A109" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A110" s="1">
+        <v>29</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A111" s="1">
+        <v>30</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A112" s="1">
+        <v>30</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A113" s="1">
+        <v>30</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>